<commit_message>
增加楼道的地图：a1、dd features stair and  elevator；2、add icon
</commit_message>
<xml_diff>
--- a/Document/Layer list and zIndex.xlsx
+++ b/Document/Layer list and zIndex.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="136">
   <si>
     <t>zIndex</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,165 +72,161 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>pointLayer</t>
+  </si>
+  <si>
+    <t>WFS</t>
+  </si>
+  <si>
+    <t>公司名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工位1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工位2</t>
+  </si>
+  <si>
+    <t>隔间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>卫生间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>pointLayer</t>
+    <t>出入口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LocationLayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectLayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>collectionLayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sld</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>js</t>
+  </si>
+  <si>
+    <t>js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检索</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收藏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drawpointlayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测距（polyline）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测距（point）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测距（绘制line）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RouteStartLayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路径规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RouteDestLayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RouteLayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Layer Group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优先度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优先度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Style From</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basemap</t>
+  </si>
+  <si>
+    <t>overmap</t>
+  </si>
+  <si>
+    <t>heatmapLayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>热力图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectmap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>WFS</t>
-  </si>
-  <si>
-    <t>公司名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工位1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工位2</t>
-  </si>
-  <si>
-    <t>隔间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫生间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>出入口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LocationLayer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>selectLayer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>collectionLayer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sld</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>js</t>
-  </si>
-  <si>
-    <t>js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>定位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>检索</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>收藏</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>drawpointlayer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>测距（polyline）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>测距（point）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>测距（绘制line）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Request</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RouteStartLayer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>路径规划</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RouteDestLayer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RouteLayer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>zIndex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Layer Group</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>优先度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>优先度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Style From</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>basemap</t>
-  </si>
-  <si>
-    <t>overmap</t>
-  </si>
-  <si>
-    <t>heatmapLayer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>热力图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>selectmap</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WFS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -384,10 +380,6 @@
   </si>
   <si>
     <t>update</t>
-  </si>
-  <si>
-    <t>layer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>楼层选择后拆分js，路径规划的style变更</t>
@@ -509,6 +501,48 @@
   </si>
   <si>
     <t>electronicFenceStyle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卫生间</t>
+  </si>
+  <si>
+    <t>ol3-style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ol3-style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电梯间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>楼梯间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>楼梯间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1.0.3</t>
+  </si>
+  <si>
+    <t>layer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>layer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加电梯和楼梯的feature和index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陈雅婷</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1321,7 +1355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -1455,69 +1489,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1526,6 +1497,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1806,13 +1845,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:K29"/>
+  <dimension ref="C1:K33"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomRight" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1833,45 +1872,45 @@
     <row r="1" spans="3:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="3:11" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="90" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="75" t="s">
+      <c r="F3" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="99"/>
+      <c r="I3" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="80"/>
+      <c r="K3" s="81"/>
+    </row>
+    <row r="4" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="91"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="95"/>
-      <c r="I3" s="75" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="76"/>
-      <c r="K3" s="77"/>
-    </row>
-    <row r="4" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="87"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="47" t="s">
+      <c r="H4" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="47" t="s">
+      <c r="I4" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="83"/>
+      <c r="K4" s="48" t="s">
         <v>46</v>
-      </c>
-      <c r="I4" s="78" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="79"/>
-      <c r="K4" s="48" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="3:11" x14ac:dyDescent="0.2">
@@ -1888,13 +1927,13 @@
         <v>6</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H5" s="6">
         <v>0</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J5" s="22"/>
       <c r="K5" s="24">
@@ -1902,7 +1941,7 @@
       </c>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C6" s="80" t="s">
+      <c r="C6" s="84" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="15">
@@ -1911,615 +1950,699 @@
       <c r="E6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="92" t="s">
+      <c r="F6" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="92" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="92">
+      <c r="G6" s="96" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="96">
         <v>10</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K6" s="16">
         <v>101</v>
       </c>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C7" s="81"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="17">
         <v>10030501</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="93"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="97"/>
       <c r="I7" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K7" s="18">
         <v>102</v>
       </c>
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C8" s="81"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="17">
         <v>10030502</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="97"/>
       <c r="I8" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K8" s="18">
         <v>102</v>
       </c>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C9" s="81"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="17">
         <v>10030504</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="97"/>
       <c r="I9" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K9" s="18">
         <v>102</v>
       </c>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C10" s="81"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="17">
         <v>10030505</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="93"/>
-      <c r="G10" s="93"/>
-      <c r="H10" s="93"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
       <c r="I10" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
       <c r="K10" s="18">
         <v>103</v>
       </c>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C11" s="82"/>
-      <c r="D11" s="19">
+      <c r="C11" s="100"/>
+      <c r="D11" s="101">
         <v>10030602</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="101" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="97"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="97"/>
+      <c r="I11" s="101" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="101" t="s">
+        <v>127</v>
+      </c>
+      <c r="K11" s="102">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C12" s="100"/>
+      <c r="D12" s="101">
+        <v>10030604</v>
+      </c>
+      <c r="E12" s="101" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="97"/>
+      <c r="G12" s="97"/>
+      <c r="H12" s="97"/>
+      <c r="I12" s="101" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="101" t="s">
+        <v>127</v>
+      </c>
+      <c r="K12" s="102">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C13" s="86"/>
+      <c r="D13" s="19">
+        <v>10030605</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="F13" s="98"/>
+      <c r="G13" s="98"/>
+      <c r="H13" s="98"/>
+      <c r="I13" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="K13" s="20">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C14" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="19" t="s">
+      <c r="D14" s="15">
+        <v>30060000</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="96" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="96">
+        <v>30</v>
+      </c>
+      <c r="I14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="K11" s="20">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C12" s="83" t="s">
+      <c r="J14" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="K14" s="16">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C15" s="88"/>
+      <c r="D15" s="17">
+        <v>30060100</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="97"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="K15" s="18">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C16" s="88"/>
+      <c r="D16" s="17">
+        <v>30060200</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="97"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="97"/>
+      <c r="I16" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="K16" s="18">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C17" s="88"/>
+      <c r="D17" s="17">
+        <v>30060300</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="97"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="K17" s="18">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C18" s="88"/>
+      <c r="D18" s="17">
+        <v>30050100</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="97"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="97"/>
+      <c r="I18" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="K18" s="18">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C19" s="88"/>
+      <c r="D19" s="101">
+        <v>30050200</v>
+      </c>
+      <c r="E19" s="101" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="97"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="97"/>
+      <c r="I19" s="101" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="101" t="s">
+        <v>127</v>
+      </c>
+      <c r="K19" s="102">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C20" s="88"/>
+      <c r="D20" s="101">
+        <v>30050300</v>
+      </c>
+      <c r="E20" s="101" t="s">
+        <v>128</v>
+      </c>
+      <c r="F20" s="97"/>
+      <c r="G20" s="97"/>
+      <c r="H20" s="97"/>
+      <c r="I20" s="101" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="101" t="s">
+        <v>127</v>
+      </c>
+      <c r="K20" s="102">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C21" s="89"/>
+      <c r="D21" s="19">
+        <v>30050800</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="98"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="98"/>
+      <c r="I21" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="K21" s="20">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C22" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="15">
-        <v>30060000</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="92" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="92" t="s">
+      <c r="G22" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H22" s="7">
+        <v>5</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="K22" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C23" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="92">
+      <c r="H23" s="8">
+        <v>60</v>
+      </c>
+      <c r="I23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="K23" s="14">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C24" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="F24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="8">
+        <v>50</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="K24" s="14">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C25" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="K12" s="16">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C13" s="84"/>
-      <c r="D13" s="17">
-        <v>30060100</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="93"/>
-      <c r="G13" s="93"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="K13" s="18">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C14" s="84"/>
-      <c r="D14" s="17">
-        <v>30060200</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="93"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="93"/>
-      <c r="I14" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="K14" s="18">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C15" s="84"/>
-      <c r="D15" s="17">
-        <v>30060300</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="93"/>
-      <c r="G15" s="93"/>
-      <c r="H15" s="93"/>
-      <c r="I15" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="K15" s="18">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C16" s="84"/>
-      <c r="D16" s="17">
-        <v>30050100</v>
-      </c>
-      <c r="E16" s="17" t="s">
+      <c r="E25" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25" s="8">
+        <v>80</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C26" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="8">
+        <v>40</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="K26" s="14">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C27" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27" s="9">
+        <v>100</v>
+      </c>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K27" s="29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C28" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H28" s="10">
+        <v>70</v>
+      </c>
+      <c r="I28" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="K28" s="16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C29" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="17"/>
+      <c r="G29" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" s="11">
+        <v>70</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="K29" s="18">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C30" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="10">
+        <v>90</v>
+      </c>
+      <c r="I30" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="K30" s="16">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C31" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" s="11">
+        <v>90</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="J31" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="K31" s="18">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="H32" s="38">
         <v>20</v>
       </c>
-      <c r="F16" s="93"/>
-      <c r="G16" s="93"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="K16" s="18">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C17" s="85"/>
-      <c r="D17" s="19">
-        <v>30050800</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="94"/>
-      <c r="G17" s="94"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="K17" s="20">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C18" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="7">
-        <v>5</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="K18" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C19" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H19" s="8">
-        <v>60</v>
-      </c>
-      <c r="I19" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="K19" s="14">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C20" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" s="8">
-        <v>50</v>
-      </c>
-      <c r="I20" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="K20" s="14">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C21" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H21" s="8">
-        <v>80</v>
-      </c>
-      <c r="I21" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="J21" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="K21" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C22" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H22" s="8">
-        <v>40</v>
-      </c>
-      <c r="I22" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="J22" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="K22" s="14">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C23" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H23" s="9">
-        <v>100</v>
-      </c>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="K23" s="29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C24" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" s="10">
-        <v>70</v>
-      </c>
-      <c r="I24" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="J24" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="K24" s="16">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C25" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H25" s="11">
-        <v>70</v>
-      </c>
-      <c r="I25" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="J25" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="K25" s="18">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C26" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H26" s="10">
+      <c r="I32" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="J32" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="I26" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="J26" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="K26" s="16">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C27" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H27" s="11">
-        <v>90</v>
-      </c>
-      <c r="I27" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="J27" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="K27" s="18">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="28" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="H28" s="38">
-        <v>20</v>
-      </c>
-      <c r="I28" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="J28" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="K28" s="40">
+      <c r="K32" s="40">
         <v>250</v>
       </c>
     </row>
-    <row r="29" spans="3:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
+    <row r="33" spans="3:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="C14:C21"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F6:F11"/>
-    <mergeCell ref="F12:F17"/>
-    <mergeCell ref="G6:G11"/>
-    <mergeCell ref="G12:G17"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="H12:H17"/>
+    <mergeCell ref="F6:F13"/>
+    <mergeCell ref="F14:F21"/>
+    <mergeCell ref="G6:G13"/>
+    <mergeCell ref="G14:G21"/>
+    <mergeCell ref="H6:H13"/>
+    <mergeCell ref="H14:H21"/>
     <mergeCell ref="G3:H3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F6 F12 F18:F29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F6 F14 F22:F33">
       <formula1>"WFS,WMS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G12 G19:G29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G14 G23:G33">
       <formula1>"basemap,overmap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I33">
       <formula1>"sld,js"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2551,34 +2674,34 @@
     <row r="2" spans="3:4" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C4" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="52" t="s">
         <v>55</v>
-      </c>
-      <c r="D4" s="52" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C5" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="56" t="s">
         <v>66</v>
-      </c>
-      <c r="D6" s="56" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7" spans="3:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2617,155 +2740,155 @@
     <row r="2" spans="3:7" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="45" t="s">
-        <v>69</v>
-      </c>
       <c r="E3" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="G3" s="50" t="s">
         <v>78</v>
-      </c>
-      <c r="G3" s="50" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="51" t="s">
+      <c r="G4" s="52" t="s">
         <v>59</v>
-      </c>
-      <c r="G4" s="52" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="54" t="s">
         <v>72</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="54" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="76" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="76" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="77" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="78" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="76" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="76" t="s">
         <v>112</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="54" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C7" s="96" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" s="97" t="s">
+      <c r="F8" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" s="78" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C9" s="75" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="76" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="G9" s="78" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C10" s="75" t="s">
         <v>118</v>
       </c>
-      <c r="E7" s="97" t="s">
-        <v>108</v>
-      </c>
-      <c r="F7" s="98" t="s">
-        <v>109</v>
-      </c>
-      <c r="G7" s="99" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C8" s="96" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" s="97" t="s">
-        <v>113</v>
-      </c>
-      <c r="E8" s="97" t="s">
-        <v>114</v>
-      </c>
-      <c r="F8" s="98" t="s">
-        <v>115</v>
-      </c>
-      <c r="G8" s="99" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C9" s="96" t="s">
+      <c r="D10" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="D9" s="97" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="97" t="s">
-        <v>122</v>
-      </c>
-      <c r="F9" s="98" t="s">
-        <v>115</v>
-      </c>
-      <c r="G9" s="99" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C10" s="96" t="s">
+      <c r="E10" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="97" t="s">
-        <v>121</v>
-      </c>
-      <c r="E10" s="97" t="s">
-        <v>122</v>
-      </c>
-      <c r="F10" s="98" t="s">
-        <v>125</v>
-      </c>
-      <c r="G10" s="99" t="s">
-        <v>126</v>
+      <c r="F10" s="77" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="78" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C11" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F11" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="G11" s="56" t="s">
         <v>124</v>
-      </c>
-      <c r="F11" s="55" t="s">
-        <v>125</v>
-      </c>
-      <c r="G11" s="56" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="12" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -2785,7 +2908,7 @@
   <dimension ref="B1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2798,91 +2921,103 @@
     <row r="1" spans="2:7" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="D2" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="E2" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="F2" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="G2" s="60" t="s">
         <v>84</v>
-      </c>
-      <c r="G2" s="60" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="D3" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="62" t="s">
-        <v>88</v>
-      </c>
       <c r="E3" s="63" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F3" s="64">
         <v>42835</v>
       </c>
       <c r="G3" s="65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="66" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C4" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="67" t="s">
         <v>93</v>
-      </c>
-      <c r="D4" s="67" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="67" t="s">
-        <v>95</v>
       </c>
       <c r="F4" s="68">
         <v>42846</v>
       </c>
       <c r="G4" s="69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="70" t="s">
         <v>103</v>
-      </c>
-      <c r="C5" s="67" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="70" t="s">
-        <v>104</v>
-      </c>
-      <c r="E5" s="70" t="s">
-        <v>105</v>
       </c>
       <c r="F5" s="68">
         <v>42872</v>
       </c>
       <c r="G5" s="69" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="66"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="69"/>
+      <c r="B6" s="66" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" s="68">
+        <v>42891</v>
+      </c>
+      <c r="G6" s="69" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="7" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="66"/>

</xml_diff>